<commit_message>
update add type question
</commit_message>
<xml_diff>
--- a/mean/public/assets/excel/template_excel_list_question.xlsx
+++ b/mean/public/assets/excel/template_excel_list_question.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>TITLE</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Câu hỏi 1</t>
   </si>
   <si>
-    <t>Điền vào chỗ trống</t>
-  </si>
-  <si>
     <t>medium</t>
   </si>
   <si>
@@ -62,6 +59,45 @@
   </si>
   <si>
     <t>mc</t>
+  </si>
+  <si>
+    <t>Chọn đáp án đúng</t>
+  </si>
+  <si>
+    <t>Chọn một đáp án đúng</t>
+  </si>
+  <si>
+    <t>Câu hỏi 3</t>
+  </si>
+  <si>
+    <t>Câu hỏi 4</t>
+  </si>
+  <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t>hard</t>
+  </si>
+  <si>
+    <t>tf</t>
+  </si>
+  <si>
+    <t>fb</t>
+  </si>
+  <si>
+    <t>0;</t>
+  </si>
+  <si>
+    <t>1;</t>
+  </si>
+  <si>
+    <t>a;an</t>
+  </si>
+  <si>
+    <t>Điền từ vào chỗ trống</t>
+  </si>
+  <si>
+    <t>are;is</t>
   </si>
 </sst>
 </file>
@@ -894,7 +930,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -902,13 +938,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -935,39 +976,79 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update template excel list question
</commit_message>
<xml_diff>
--- a/mean/public/assets/excel/template_excel_list_question.xlsx
+++ b/mean/public/assets/excel/template_excel_list_question.xlsx
@@ -19,9 +19,6 @@
     <t>TITLE</t>
   </si>
   <si>
-    <t>CONTENT</t>
-  </si>
-  <si>
     <t>LEVEL</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>are;is</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -930,7 +930,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -941,7 +941,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -956,99 +956,99 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>